<commit_message>
Update to version v6.0.2
</commit_message>
<xml_diff>
--- a/.nightswatch/functional/files/import-pass.xlsx
+++ b/.nightswatch/functional/files/import-pass.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mburnie/workplace/nightswatch/src/NightsWatchSolutions/source/solutions-nightswatch-tests/qnabot-on-aws/regression-tests/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikemlin/f-team/awsaiml/src/Aws-ai-qna-bot/.nightswatch/functional/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E949002-E97E-9D4D-BE0F-260ECC40D5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6032812A-491A-AC4B-A9D9-F98DDBEBAB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{65063F85-4105-8F42-BAD0-641D55AA808E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17660" xr2:uid="{65063F85-4105-8F42-BAD0-641D55AA808E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>qid</t>
   </si>
@@ -157,6 +157,15 @@
   </si>
   <si>
     <t>Can I import multiple answers when I import with excel using QnA Bot?</t>
+  </si>
+  <si>
+    <t>今日は晴れです。</t>
+  </si>
+  <si>
+    <t>DoubleByteCharacters.001</t>
+  </si>
+  <si>
+    <t>今日の天気を教えてください.</t>
   </si>
 </sst>
 </file>
@@ -543,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654EBFE9-4F2B-8349-985B-01DDB193FC33}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -701,6 +710,18 @@
         <v>40</v>
       </c>
     </row>
+    <row r="4" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" xr:uid="{32E63726-E902-C741-9B4E-0BDC2DAE7EF6}"/>

</xml_diff>